<commit_message>
actor and movie data deleted, fifa eu gs jana as csv
</commit_message>
<xml_diff>
--- a/Gold Standard/goldstandard_Jana.xlsx
+++ b/Gold Standard/goldstandard_Jana.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067608\Documents\MMDS Masterstudium Unterlagen\Semester I\Web Data Integration\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D067608\Documents\WDI_2019\Gold Standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CAE934-0756-44B8-A8A1-D4E490AEAEAE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831EA686-6A89-4045-BB08-5D4536B61421}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E2D2A58-07B2-4AEB-B295-0EE689D62951}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1E2D2A58-07B2-4AEB-B295-0EE689D62951}"/>
   </bookViews>
   <sheets>
     <sheet name="FIFA-ESD" sheetId="1" r:id="rId1"/>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F2854C-0B7C-4DD8-B457-2C08A7DD72A1}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2145,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB954655-3A23-44DA-A094-F4A7922CFB59}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>

</xml_diff>